<commit_message>
Successfully converted to Maven
</commit_message>
<xml_diff>
--- a/src/Test data.xlsx
+++ b/src/Test data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t xml:space="preserve">Login</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>000001514520710375</t>
+  </si>
+  <si>
+    <t>000001514994117116</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">

</xml_diff>

<commit_message>
xml file undate in pom
</commit_message>
<xml_diff>
--- a/src/Test data.xlsx
+++ b/src/Test data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve">Login</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>000001515047221824</t>
+  </si>
+  <si>
+    <t>000001515085186596</t>
+  </si>
+  <si>
+    <t>000001515240526631</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">

</xml_diff>

<commit_message>
Separated Staging and Prod code
</commit_message>
<xml_diff>
--- a/src/Test data.xlsx
+++ b/src/Test data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t xml:space="preserve">Login</t>
   </si>
@@ -93,9 +93,15 @@
     <t xml:space="preserve">Admin:</t>
   </si>
   <si>
+    <t xml:space="preserve">SignUp</t>
+  </si>
+  <si>
     <t xml:space="preserve">sumit.testmail02@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Automated</t>
+  </si>
+  <si>
     <t xml:space="preserve">pass</t>
   </si>
   <si>
@@ -108,7 +114,10 @@
     <t xml:space="preserve">order</t>
   </si>
   <si>
-    <t xml:space="preserve">000001515037609267</t>
+    <t xml:space="preserve">000001515451964929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sumit+3@circles.asia</t>
   </si>
   <si>
     <t xml:space="preserve">pincode</t>
@@ -201,13 +210,22 @@
     <t xml:space="preserve">https://kirk.circles.asia:7443</t>
   </si>
   <si>
-    <t>000001515047221824</t>
-  </si>
-  <si>
-    <t>000001515085186596</t>
-  </si>
-  <si>
-    <t>000001515240526631</t>
+    <t>000001515733066346</t>
+  </si>
+  <si>
+    <t>000001515733350807</t>
+  </si>
+  <si>
+    <t>000001515738960875</t>
+  </si>
+  <si>
+    <t>000001515739167985</t>
+  </si>
+  <si>
+    <t>000001515739308951</t>
+  </si>
+  <si>
+    <t>000001515739568617</t>
   </si>
 </sst>
 </file>
@@ -584,10 +602,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+      <selection activeCell="F12" activeCellId="0" pane="topLeft" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -595,7 +613,7 @@
     <col min="1" max="1" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="20.27" collapsed="true" outlineLevel="0"/>
     <col min="3" max="3" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="35.33" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="22.13" collapsed="true" outlineLevel="0"/>
     <col min="5" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
@@ -607,13 +625,16 @@
       <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -621,87 +642,99 @@
       <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="3">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>88001572</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>600340</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.55" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>98818812</v>
@@ -709,7 +742,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>4111111111111110</v>
@@ -717,7 +750,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>965</v>
@@ -725,16 +758,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="sumit.testmail02@gmail.com" r:id="rId1" ref="B2"/>
     <hyperlink display="sumit@circles.asia" r:id="rId2" ref="D2"/>
+    <hyperlink display="sumit+3@circles.asia" r:id="rId3" ref="E4"/>
   </hyperlinks>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
@@ -764,59 +798,59 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Biling Automation code and refrctory code
</commit_message>
<xml_diff>
--- a/src/Test data.xlsx
+++ b/src/Test data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t xml:space="preserve">Login</t>
   </si>
@@ -64,27 +64,13 @@
     <t xml:space="preserve">Kirk pass</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF808080"/>
-        <rFont val="Monaco"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sumit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF808080"/>
-        <rFont val="Monaco"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">@circles@12</t>
-    </r>
+    <t xml:space="preserve">crestelpass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sumit2circle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testCrestel</t>
   </si>
   <si>
     <t xml:space="preserve">Website</t>
@@ -111,7 +97,7 @@
     <t xml:space="preserve">order</t>
   </si>
   <si>
-    <t xml:space="preserve">000001517279228067</t>
+    <t xml:space="preserve">000001518501622891</t>
   </si>
   <si>
     <t xml:space="preserve">sumit+3@circles.asia</t>
@@ -165,6 +151,9 @@
     <t xml:space="preserve">Sumit</t>
   </si>
   <si>
+    <t xml:space="preserve">promo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Staging Auth url:</t>
   </si>
   <si>
@@ -205,6 +194,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://kirk.circles.asia:7443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testbed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://testliberty.crestelbss.om.com:9080/index.zul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crestel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://libertywireless.crestelbss.om.com:9080/index.zul</t>
   </si>
 </sst>
 </file>
@@ -259,13 +260,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF808080"/>
-      <name val="Monaco"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -282,6 +276,13 @@
       <sz val="12"/>
       <color rgb="FF353535"/>
       <name val="AppleSystemUIFont"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Monaco"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -365,19 +366,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,10 +510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -552,12 +553,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +598,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -598,14 +615,14 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,98 +639,98 @@
         <v>5</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>88001572</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>600340</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="32.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>98818812</v>
@@ -721,7 +738,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>4111111111111110</v>
@@ -729,7 +746,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>965</v>
@@ -737,10 +754,15 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -764,10 +786,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -777,59 +799,75 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated app code also.
</commit_message>
<xml_diff>
--- a/src/Test data.xlsx
+++ b/src/Test data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="165">
   <si>
     <t xml:space="preserve">Login</t>
   </si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">order</t>
   </si>
   <si>
-    <t xml:space="preserve">000001518501622891</t>
+    <t xml:space="preserve">test</t>
   </si>
   <si>
     <t xml:space="preserve">sumit+3@circles.asia</t>
@@ -107,6 +107,12 @@
     <t xml:space="preserve">pincode</t>
   </si>
   <si>
+    <t xml:space="preserve">CHANDRA TEST DB MIGRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/08/2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">house</t>
   </si>
   <si>
@@ -119,6 +125,9 @@
     <t xml:space="preserve">Automation Street</t>
   </si>
   <si>
+    <t xml:space="preserve">Phyoe Phyoe</t>
+  </si>
+  <si>
     <t xml:space="preserve">unit</t>
   </si>
   <si>
@@ -209,10 +218,307 @@
     <t xml:space="preserve">http://libertywireless.crestelbss.om.com:9080/index.zul</t>
   </si>
   <si>
+    <t xml:space="preserve">banumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW1618883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW130898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sinumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW1618885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkoutdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-11-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addresss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123A, test building name, test street name Unit 01-234 test building name, test street name;;01-234;123A, Singapore, Singapore, Singapore, 159557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobilenumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87421420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW1618884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bacustomeremail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ritesh@circles.asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW130897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW1618882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customerpincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">426402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refcodeused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RITESH BATRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customeradd2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">221 henderson road;2nd floor;221;221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customeridtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customeradd1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">221, 221 henderson road, #2nd floor-221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customercountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singapore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">earliestterm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-03-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bacustomername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sicustomername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW130899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customeridnumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXXXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW130900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customeremail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customerdob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1987-04-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customercity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sicustomeremail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">planswitchdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roamingcap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ 100</t>
+  </si>
+  <si>
+    <t>banumber</t>
+  </si>
+  <si>
+    <t>LW1618883</t>
+  </si>
+  <si>
+    <t>checkoutdate</t>
+  </si>
+  <si>
+    <t>2017-08-30</t>
+  </si>
+  <si>
+    <t>mobilenumber</t>
+  </si>
+  <si>
+    <t>87423620</t>
+  </si>
+  <si>
+    <t>bacustomeremail</t>
+  </si>
+  <si>
+    <t>sumit@circles.asia</t>
+  </si>
+  <si>
+    <t>canumber</t>
+  </si>
+  <si>
+    <t>LW1618882</t>
+  </si>
+  <si>
+    <t>customerpincode</t>
+  </si>
+  <si>
+    <t>159557</t>
+  </si>
+  <si>
+    <t>refcodeused</t>
+  </si>
+  <si>
+    <t>BTXUD</t>
+  </si>
+  <si>
+    <t>orderref</t>
+  </si>
+  <si>
+    <t>000001504046868726</t>
+  </si>
+  <si>
+    <t>customername</t>
+  </si>
+  <si>
     <t>CHANDRA TEST DB MIGRATION</t>
   </si>
   <si>
-    <t>30/08/2017</t>
+    <t>customeradd2</t>
+  </si>
+  <si>
+    <t>Henderson road;;6-10;221</t>
+  </si>
+  <si>
+    <t>customeridtype</t>
+  </si>
+  <si>
+    <t>NRIC</t>
+  </si>
+  <si>
+    <t>customeradd1</t>
+  </si>
+  <si>
+    <t>221, Henderson road</t>
+  </si>
+  <si>
+    <t>customercountry</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>earliestterm</t>
+  </si>
+  <si>
+    <t>2018-03-31</t>
+  </si>
+  <si>
+    <t>bacustomername</t>
+  </si>
+  <si>
+    <t>sicustomername</t>
+  </si>
+  <si>
+    <t>sanumber</t>
+  </si>
+  <si>
+    <t>LW1618884</t>
+  </si>
+  <si>
+    <t>customeridnumber</t>
+  </si>
+  <si>
+    <t>G1381300R</t>
+  </si>
+  <si>
+    <t>sinumber</t>
+  </si>
+  <si>
+    <t>LW1618885</t>
+  </si>
+  <si>
+    <t>customeremail</t>
+  </si>
+  <si>
+    <t>customerdob</t>
+  </si>
+  <si>
+    <t>1989-10-30</t>
+  </si>
+  <si>
+    <t>customercity</t>
+  </si>
+  <si>
+    <t>sicustomeremail</t>
+  </si>
+  <si>
+    <t>planswitchdate</t>
+  </si>
+  <si>
+    <t>roamingcap</t>
+  </si>
+  <si>
+    <t>$ 100</t>
+  </si>
+  <si>
+    <t>addresss</t>
+  </si>
+  <si>
+    <t>123A, test building name, test street name Unit 01-234 test building name, test street name;;01-234;123A, Singapore, Singapore, Singapore, 159557</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -222,7 +528,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -269,12 +575,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -336,7 +636,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -381,11 +681,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -468,7 +764,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
       <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -519,7 +815,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
       <selection activeCell="C7" activeCellId="0" pane="topLeft" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -605,10 +901,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
+      <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
@@ -690,92 +986,225 @@
       <c r="B5" s="1" t="n">
         <v>600340</v>
       </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
+      <c r="D5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.55" outlineLevel="0" r="10">
+        <v>37</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.25" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>98818812</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>4111111111111110</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>965</v>
       </c>
+      <c r="C13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+      <c r="C16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
+      <c r="C17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
+      <c r="C18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19">
+      <c r="C19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
+      <c r="C20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
+      <c r="C21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22">
+      <c r="C22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="23">
+      <c r="C23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
+      <c r="C24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="25">
+      <c r="C25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +1230,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
       <selection activeCell="B14" activeCellId="0" pane="topLeft" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -812,75 +1241,75 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -907,17 +1336,266 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="49" zoomScaleNormal="49" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
+      <selection activeCell="E18" activeCellId="0" pane="topLeft" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="1" max="3" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="15.92" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="17.94" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+      <c r="B8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+      <c r="D9" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+      <c r="D10" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+      <c r="D11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
+      <c r="D12" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
+      <c r="D13" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
+      <c r="D14" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
+      <c r="D15" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+      <c r="D16" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
+      <c r="D17" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
+      <c r="D18" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19">
+      <c r="D19" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
+      <c r="D20" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
+      <c r="D21" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22">
+      <c r="D22" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="23">
+      <c r="D23" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
+      <c r="D24" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="25">
+      <c r="D25" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>

</xml_diff>